<commit_message>
update modules of xls
</commit_message>
<xml_diff>
--- a/static/excel/业绩指标模版.xlsx
+++ b/static/excel/业绩指标模版.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ypzhuang/work/projects/vue_projects/pig-ui/static/excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\阿熙\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{90434F9B-E8CE-8E4F-87D1-18C17F700A38}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C23902F-33D2-48DE-A27A-ACF1136A920F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9024" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="业绩指标" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="150001"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -213,7 +213,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="176" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -308,7 +308,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -326,19 +326,23 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -619,28 +623,28 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <cols>
-    <col min="2" max="2" width="17.33203125" customWidth="1"/>
-    <col min="3" max="3" width="16.1640625" customWidth="1"/>
-    <col min="4" max="4" width="33.5" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="20.33203125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="17.36328125" style="16" customWidth="1"/>
+    <col min="3" max="3" width="16.1796875" style="16" customWidth="1"/>
+    <col min="4" max="4" width="33.453125" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="6" max="6" width="12.6328125" customWidth="1"/>
+    <col min="7" max="7" width="20.36328125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17">
+    <row r="1" spans="1:7" ht="17.399999999999999">
       <c r="A1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
       <c r="D1" s="6"/>
     </row>
-    <row r="2" spans="1:7" ht="19">
+    <row r="2" spans="1:7" ht="20.399999999999999">
       <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
@@ -648,7 +652,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:7" ht="19">
+    <row r="3" spans="1:7" ht="20.399999999999999">
       <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
@@ -656,19 +660,27 @@
       <c r="C3" s="5"/>
       <c r="D3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="20">
+    <row r="4" spans="1:7" ht="20.399999999999999">
+      <c r="B4"/>
+      <c r="C4"/>
       <c r="D4" s="7"/>
       <c r="E4" s="7"/>
       <c r="F4" s="7"/>
       <c r="G4" s="8"/>
     </row>
     <row r="5" spans="1:7">
+      <c r="B5"/>
+      <c r="C5"/>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
       <c r="F5" s="9"/>
       <c r="G5" s="10"/>
     </row>
-    <row r="7" spans="1:7" ht="20">
+    <row r="6" spans="1:7">
+      <c r="B6"/>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.399999999999999">
       <c r="A7" s="11" t="s">
         <v>42</v>
       </c>
@@ -728,7 +740,7 @@
       <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15.6"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" s="2" t="s">

</xml_diff>